<commit_message>
latest update date 6th June 2021
</commit_message>
<xml_diff>
--- a/main/.data/momentum/[2021][HuyNguyen]-TradingView.xlsx
+++ b/main/.data/momentum/[2021][HuyNguyen]-TradingView.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>DAY</t>
   </si>
@@ -92,18 +92,6 @@
   </si>
   <si>
     <t>commnet</t>
-  </si>
-  <si>
-    <t>GBPUSD</t>
-  </si>
-  <si>
-    <t>16:15</t>
-  </si>
-  <si>
-    <t>https://www.tradingview.com/x/AOKAebW8/</t>
-  </si>
-  <si>
-    <t>1 comment</t>
   </si>
 </sst>
 </file>
@@ -453,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -588,38 +576,6 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1.45</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1.45</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A3"/>
@@ -628,8 +584,6 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1"/>
     <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>